<commit_message>
added YouTube link to ReadMe
</commit_message>
<xml_diff>
--- a/App Flow Diagram.xlsx
+++ b/App Flow Diagram.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelcouch/Documents/CODE/react_testing/strike_api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35AD3E66-82AF-F24E-B988-E364341688D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE47A5DC-3F42-AE4B-896A-CC07D84CEE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32760" yWindow="1380" windowWidth="27160" windowHeight="18520" xr2:uid="{267C899B-033C-FC44-8B73-C256A7A2A341}"/>
+    <workbookView xWindow="1860" yWindow="920" windowWidth="23220" windowHeight="14600" xr2:uid="{267C899B-033C-FC44-8B73-C256A7A2A341}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>User</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>Strike API</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -2533,7 +2536,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEEFD6EF-1926-C94A-A910-4C3353B622B8}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H35" sqref="H35"/>
@@ -2559,6 +2562,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="35" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H35" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>